<commit_message>
Ausdrucken von EXCEL eCH-0160_xIsadg&EAD_v2.1.xlsx verbessert
</commit_message>
<xml_diff>
--- a/DataDictionary/eCH-0160_xIsadg&EAD_v2.1.xlsx
+++ b/DataDictionary/eCH-0160_xIsadg&EAD_v2.1.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="5970" windowWidth="10230" windowHeight="1725" tabRatio="861"/>
+    <workbookView xWindow="-15" yWindow="5970" windowWidth="10230" windowHeight="1725" tabRatio="861" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="eCH-0160 zu xIsadg v1.6.1" sheetId="13" r:id="rId1"/>
@@ -22,7 +22,7 @@
     <definedName name="_ftnref2" localSheetId="2">xIsadg_DataDictionary!#REF!</definedName>
     <definedName name="_ftnref3" localSheetId="2">xIsadg_DataDictionary!#REF!</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'eCH-0160 zu xIsadg v1.6.1'!$A$1:$J$42</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">'eCH-0160 zu xIsadg v2.1'!$A$1:$L$68</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">'eCH-0160 zu xIsadg v2.1'!$A$1:$N$68</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="2">xIsadg_DataDictionary!$A$1:$H$41</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="2">xIsadg_DataDictionary!$2:$2</definedName>
     <definedName name="OLE_LINK3" localSheetId="2">xIsadg_DataDictionary!#REF!</definedName>
@@ -3389,7 +3389,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="33">
     <font>
       <sz val="10"/>
@@ -5457,7 +5457,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -5748,7 +5748,7 @@
   </sheetPr>
   <dimension ref="A1:J115"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection sqref="A1:J1"/>
     </sheetView>
   </sheetViews>
@@ -6827,8 +6827,8 @@
   </sheetPr>
   <dimension ref="A1:M75"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="M53" sqref="M53"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="58.7109375" defaultRowHeight="12.75"/>
@@ -6845,7 +6845,9 @@
     <col min="10" max="10" width="4.140625" style="171" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="27" style="171" customWidth="1"/>
     <col min="12" max="12" width="27.42578125" style="171" customWidth="1"/>
-    <col min="13" max="16384" width="58.7109375" style="145"/>
+    <col min="13" max="13" width="58.7109375" style="145"/>
+    <col min="14" max="14" width="32.28515625" style="145" customWidth="1"/>
+    <col min="15" max="16384" width="58.7109375" style="145"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="29.25" customHeight="1" thickBot="1">
@@ -8115,8 +8117,8 @@
     </cfRule>
   </conditionalFormatting>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
-  <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.39370078740157483" bottom="0.39370078740157483" header="0.31496062992125984" footer="0.23622047244094491"/>
-  <pageSetup paperSize="9" scale="41" orientation="landscape" r:id="rId1"/>
+  <pageMargins left="0.15748031496062992" right="7.874015748031496E-2" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup paperSize="8" scale="48" fitToHeight="0" orientation="landscape" cellComments="asDisplayed" r:id="rId1"/>
   <headerFooter>
     <oddFooter>&amp;L&amp;F&amp;R2</oddFooter>
   </headerFooter>

</xml_diff>

<commit_message>
Existenzzeitraum und Anwendungszeitraum ein Datumsfeld und kein Textfeld in xIsadg v2.1
</commit_message>
<xml_diff>
--- a/DataDictionary/eCH-0160_xIsadg&EAD_v2.1.xlsx
+++ b/DataDictionary/eCH-0160_xIsadg&EAD_v2.1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\KOST\Standards\xIsadg\01_workbench\DataDictionary\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\KOST\Standards\xIsadg\_Workbench\DataDictionary\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1017,7 +1017,7 @@
             <rFont val="Segoe UI"/>
             <family val="2"/>
           </rPr>
-          <t>Existenzzeitraum ist ein Textfeld und kein Datumsfeld, weil es nur den Status von Kommentar hat</t>
+          <t>Existenzzeitraum ist ein Datumsfeld aber kein "date" im Sinne von ISAD(G) weil es nur den Status von Kommentar hat</t>
         </r>
       </text>
     </comment>
@@ -1194,7 +1194,7 @@
             <rFont val="Segoe UI"/>
             <family val="2"/>
           </rPr>
-          <t>Anwendungszeitraum ist ein Textfeld und kein Datumsfeld, weil es nur den Status von Kommentar hat</t>
+          <t>Anwendungszeitraum  ist ein Datumsfeld aber kein "date" im Sinne von ISAD(G) weil es nur den Status von Kommentar hat</t>
         </r>
       </text>
     </comment>
@@ -6828,7 +6828,7 @@
   <dimension ref="A1:M75"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+      <selection sqref="A1:L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="58.7109375" defaultRowHeight="12.75"/>

</xml_diff>